<commit_message>
minor edit to xls file
</commit_message>
<xml_diff>
--- a/R_MultiAssayExperiment/mae_example_data.xlsx
+++ b/R_MultiAssayExperiment/mae_example_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16120" yWindow="5500" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="16120" yWindow="5500" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="clindata" sheetId="1" r:id="rId1"/>
@@ -703,8 +703,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -735,15 +743,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -751,31 +765,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1127,29 +1161,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1222,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1233,79 +1268,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>219</v>
       </c>
     </row>
@@ -1325,7 +1360,7 @@
   <dimension ref="A1:D199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4132,7 +4167,7 @@
   <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>